<commit_message>
verified against MAGMA up to liquid convergence check
</commit_message>
<xml_diff>
--- a/data/MAGMA_Thermodynamic_Data.xlsx
+++ b/data/MAGMA_Thermodynamic_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/PycharmProjects/MAGMApy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/Documents - Scott’s MacBook Pro/PhD Research/MAGMApy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D739E29-741A-9942-A233-70F958CA1D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A51F153E-397D-5948-A8A9-4004D6863761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10780" yWindow="760" windowWidth="26660" windowHeight="15780" activeTab="2" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
+    <workbookView xWindow="7900" yWindow="760" windowWidth="26660" windowHeight="15780" activeTab="2" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="137">
   <si>
     <t>R1</t>
   </si>
@@ -441,6 +441,12 @@
   </si>
   <si>
     <t>K2Si4O9</t>
+  </si>
+  <si>
+    <t>Fe2O3</t>
+  </si>
+  <si>
+    <t>K39</t>
   </si>
 </sst>
 </file>
@@ -1888,11 +1894,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575B768E-B263-7849-9255-8DC0D8CFF25A}">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2737,6 +2743,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>136</v>
+      </c>
+      <c r="B40" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working on gas model debugging
</commit_message>
<xml_diff>
--- a/data/MAGMA_Thermodynamic_Data.xlsx
+++ b/data/MAGMA_Thermodynamic_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/Documents - Scott’s MacBook Pro/PhD Research/MAGMApy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/PycharmProjects/MAGMApy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D753D0B6-798B-A442-8795-005E8690C28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF56BE69-19FE-8D41-A1DA-E9C0C7DEAB7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7740" yWindow="500" windowWidth="21060" windowHeight="15960" activeTab="3" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
+    <workbookView xWindow="23400" yWindow="2680" windowWidth="27460" windowHeight="17980" activeTab="3" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="168">
   <si>
     <t>R1</t>
   </si>
@@ -526,6 +526,21 @@
   </si>
   <si>
     <t>K+</t>
+  </si>
+  <si>
+    <t>Si_g</t>
+  </si>
+  <si>
+    <t>SiO2_g</t>
+  </si>
+  <si>
+    <t>Reactants</t>
+  </si>
+  <si>
+    <t>Si_l, O2_g</t>
+  </si>
+  <si>
+    <t>Si_l</t>
   </si>
 </sst>
 </file>
@@ -885,7 +900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA51B45C-F7CC-3B41-AC8C-EF614A95CDBA}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
@@ -2860,15 +2875,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1716CC3-50ED-4F4B-B9E3-816FAA8C5A11}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2881,8 +2896,11 @@
       <c r="D1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2896,201 +2914,207 @@
         <v>38621</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="C3">
-        <v>-12.56</v>
+        <v>-1.44</v>
       </c>
       <c r="D3">
-        <v>46992</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>18326</v>
+      </c>
+      <c r="E3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>114</v>
+        <v>163</v>
       </c>
       <c r="C4">
-        <v>1.19</v>
+        <v>6</v>
       </c>
       <c r="D4">
-        <v>-3794</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>-20919</v>
+      </c>
+      <c r="E4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5">
-        <v>-12.06</v>
+        <v>-12.56</v>
       </c>
       <c r="D5">
-        <v>44992</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>46992</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="C6">
-        <v>-6.35</v>
+        <v>1.19</v>
       </c>
       <c r="D6">
-        <v>19704</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>-3794</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C7">
-        <v>-2.96</v>
+        <v>-12.06</v>
       </c>
       <c r="D7">
-        <v>9753</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>44992</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8">
+        <v>-6.35</v>
+      </c>
+      <c r="D8">
+        <v>19704</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9">
+        <v>-2.96</v>
+      </c>
+      <c r="D9">
+        <v>9753</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>142</v>
       </c>
-      <c r="C8">
+      <c r="C10">
         <v>-2.26722053113</v>
       </c>
-      <c r="D8">
+      <c r="D10">
         <f>7.56430936141329*10^4</f>
         <v>75643.0936141329</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C9">
-        <v>-11.88</v>
-      </c>
-      <c r="D9">
-        <v>49586</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>144</v>
-      </c>
-      <c r="C10">
-        <v>-1.61</v>
-      </c>
-      <c r="D10">
-        <v>6128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C11">
-        <v>-33.83</v>
+        <v>-11.88</v>
       </c>
       <c r="D11">
-        <v>153255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>49586</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C12">
-        <v>-5.7</v>
+        <v>-1.61</v>
       </c>
       <c r="D12">
-        <v>15862</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C13">
-        <v>-2.66</v>
+        <v>-33.83</v>
       </c>
       <c r="D13">
-        <v>13719</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>153255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C14">
-        <v>-5.79</v>
+        <v>-5.7</v>
       </c>
       <c r="D14">
-        <v>15867.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>15862</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C15">
-        <v>-12.93</v>
+        <v>-2.66</v>
       </c>
       <c r="D15">
-        <v>54745</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13719</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C16">
-        <v>4.3099999999999996</v>
+        <v>-5.79</v>
       </c>
       <c r="D16">
-        <v>-2101</v>
+        <v>15867.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -3098,13 +3122,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C17">
-        <v>-6.46</v>
+        <v>-12.93</v>
       </c>
       <c r="D17">
-        <v>23025</v>
+        <v>54745</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -3112,13 +3136,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C18">
-        <v>-21.07</v>
+        <v>4.3099999999999996</v>
       </c>
       <c r="D18">
-        <v>95362</v>
+        <v>-2101</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -3126,13 +3150,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C19">
-        <v>-0.41</v>
+        <v>-6.46</v>
       </c>
       <c r="D19">
-        <v>17926</v>
+        <v>23025</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3140,13 +3164,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C20">
-        <v>-15.56</v>
+        <v>-21.07</v>
       </c>
       <c r="D20">
-        <v>40286</v>
+        <v>95362</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -3154,13 +3178,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C21">
-        <v>-4.9000000000000004</v>
+        <v>-0.41</v>
       </c>
       <c r="D21">
-        <v>14569</v>
+        <v>17926</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3168,13 +3192,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C22">
-        <v>-4.3099999999999996</v>
+        <v>-15.56</v>
       </c>
       <c r="D22">
-        <v>4281</v>
+        <v>40286</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3182,13 +3206,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C23">
-        <v>-10.47</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="D23">
-        <v>25180</v>
+        <v>14569</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -3196,13 +3220,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C24">
-        <v>2.8</v>
+        <v>-4.3099999999999996</v>
       </c>
       <c r="D24">
-        <v>-27851</v>
+        <v>4281</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -3210,13 +3234,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C25">
-        <v>-15.33</v>
+        <v>-10.47</v>
       </c>
       <c r="D25">
-        <v>36735</v>
+        <v>25180</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -3224,13 +3248,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C26">
-        <v>-4.75</v>
+        <v>2.8</v>
       </c>
       <c r="D26">
-        <v>14241</v>
+        <v>-27851</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3238,13 +3262,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C27">
-        <v>-3.94</v>
+        <v>-15.33</v>
       </c>
       <c r="D27">
-        <v>2852</v>
+        <v>36735</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -3252,12 +3276,40 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>160</v>
+      </c>
+      <c r="C28">
+        <v>-4.75</v>
+      </c>
+      <c r="D28">
+        <v>14241</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>161</v>
+      </c>
+      <c r="C29">
+        <v>-3.94</v>
+      </c>
+      <c r="D29">
+        <v>2852</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
         <v>162</v>
       </c>
-      <c r="C28">
+      <c r="C30">
         <v>2.76</v>
       </c>
-      <c r="D28">
+      <c r="D30">
         <v>-23760</v>
       </c>
     </row>

</xml_diff>

<commit_message>
apparantly working gas model
</commit_message>
<xml_diff>
--- a/data/MAGMA_Thermodynamic_Data.xlsx
+++ b/data/MAGMA_Thermodynamic_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/PycharmProjects/MAGMApy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1A83743-CEE9-1D4B-AC4D-D3E7229F52D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC74446D-37A0-BC4C-BFF9-4A801360E815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18400" yWindow="4520" windowWidth="25580" windowHeight="16900" activeTab="3" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
+    <workbookView xWindow="23460" yWindow="5700" windowWidth="25580" windowHeight="16900" activeTab="3" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="179">
   <si>
     <t>R1</t>
   </si>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t>Mg_g, O</t>
+  </si>
+  <si>
+    <t>Ti, O</t>
   </si>
 </sst>
 </file>
@@ -2908,7 +2911,7 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3140,7 +3143,7 @@
         <v>145</v>
       </c>
       <c r="C15">
-        <v>-33.83</v>
+        <v>-35.83</v>
       </c>
       <c r="D15">
         <v>153255</v>
@@ -3262,6 +3265,9 @@
       </c>
       <c r="D23">
         <v>95362</v>
+      </c>
+      <c r="E23" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Trouble with gas stoich
</commit_message>
<xml_diff>
--- a/data/MAGMA_Thermodynamic_Data.xlsx
+++ b/data/MAGMA_Thermodynamic_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/Documents - Scott’s MacBook Pro/PhD Research/MAGMApy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E87ACBE-9D6A-7E4D-9847-C3B24769FF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA03FC9-25A0-3049-800D-E3310B1D2AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10440" yWindow="500" windowWidth="21560" windowHeight="15960" activeTab="3" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
+    <workbookView xWindow="13020" yWindow="500" windowWidth="15780" windowHeight="15960" activeTab="3" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="186">
   <si>
     <t>R1</t>
   </si>
@@ -540,9 +540,6 @@
     <t>Si_l</t>
   </si>
   <si>
-    <t>Si_l, O2</t>
-  </si>
-  <si>
     <t>Al2O_g</t>
   </si>
   <si>
@@ -552,9 +549,6 @@
     <t>R0</t>
   </si>
   <si>
-    <t>Fe, O</t>
-  </si>
-  <si>
     <t>Ca, O</t>
   </si>
   <si>
@@ -570,13 +564,37 @@
     <t>K2_g</t>
   </si>
   <si>
-    <t>Mg_g, O</t>
-  </si>
-  <si>
     <t>Ti, O</t>
   </si>
   <si>
     <t>Fe3O4_l</t>
+  </si>
+  <si>
+    <t>0.5*O2</t>
+  </si>
+  <si>
+    <t>1*SiO, 0.5*O2</t>
+  </si>
+  <si>
+    <t>1*SiO, -0.5*O2</t>
+  </si>
+  <si>
+    <t>1*Si_l, 1*O2</t>
+  </si>
+  <si>
+    <t>1*Si_l</t>
+  </si>
+  <si>
+    <t>1*MgO,-0.5*O2</t>
+  </si>
+  <si>
+    <t>1*Mg_g, 1*O</t>
+  </si>
+  <si>
+    <t>1*Fe, 1*O</t>
+  </si>
+  <si>
+    <t>1*Fe_g</t>
   </si>
 </sst>
 </file>
@@ -2914,7 +2932,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2938,7 +2956,7 @@
     </row>
     <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" t="s">
         <v>82</v>
@@ -2950,7 +2968,7 @@
         <v>-13282</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2966,6 +2984,9 @@
       <c r="D3">
         <v>38621</v>
       </c>
+      <c r="E3" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2980,6 +3001,9 @@
       <c r="D4">
         <v>-8207</v>
       </c>
+      <c r="E4" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -2995,7 +3019,7 @@
         <v>18326</v>
       </c>
       <c r="E5" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -3012,7 +3036,7 @@
         <v>-20919</v>
       </c>
       <c r="E6" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -3028,6 +3052,9 @@
       <c r="D7">
         <v>-3794</v>
       </c>
+      <c r="E7" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -3043,7 +3070,7 @@
         <v>46992</v>
       </c>
       <c r="E8" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -3060,7 +3087,7 @@
         <v>44992</v>
       </c>
       <c r="E9" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -3076,6 +3103,9 @@
       <c r="D10">
         <v>19704</v>
       </c>
+      <c r="E10" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -3112,7 +3142,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C13">
         <f>-3.19907301154*10^1</f>
@@ -3137,7 +3167,7 @@
         <v>49586</v>
       </c>
       <c r="E14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -3168,7 +3198,7 @@
         <v>153255</v>
       </c>
       <c r="E16" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -3204,7 +3234,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C19">
         <v>-9.36</v>
@@ -3269,7 +3299,7 @@
         <v>-2101</v>
       </c>
       <c r="E23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -3286,7 +3316,7 @@
         <v>95362</v>
       </c>
       <c r="E24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -3303,7 +3333,7 @@
         <v>17926</v>
       </c>
       <c r="E25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -3320,7 +3350,7 @@
         <v>40286</v>
       </c>
       <c r="E26" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -3337,7 +3367,7 @@
         <v>14569</v>
       </c>
       <c r="E27" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -3368,7 +3398,7 @@
         <v>25180</v>
       </c>
       <c r="E29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -3399,7 +3429,7 @@
         <v>36735</v>
       </c>
       <c r="E31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -3416,7 +3446,7 @@
         <v>14241</v>
       </c>
       <c r="E32" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -3433,7 +3463,7 @@
         <v>44099</v>
       </c>
       <c r="E33" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -3441,7 +3471,7 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C34">
         <v>-3.94</v>

</xml_diff>

<commit_message>
working gas model with spreadsheet stoich
</commit_message>
<xml_diff>
--- a/data/MAGMA_Thermodynamic_Data.xlsx
+++ b/data/MAGMA_Thermodynamic_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/Documents - Scott’s MacBook Pro/PhD Research/MAGMApy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A3E718-B3BF-7F4E-A305-C6E0B674E86E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC3705C-30BE-9242-8681-A28999E064CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="500" windowWidth="15780" windowHeight="15960" activeTab="3" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
+    <workbookView xWindow="11160" yWindow="500" windowWidth="28800" windowHeight="15960" activeTab="3" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="203">
   <si>
     <t>R1</t>
   </si>
@@ -576,24 +576,9 @@
     <t>1*Fe, 1*O</t>
   </si>
   <si>
-    <t>1*Fe_g</t>
-  </si>
-  <si>
-    <t>1*Fe_g, 0.5*O2</t>
-  </si>
-  <si>
-    <t>2*Fe_g, 1.5*O2</t>
-  </si>
-  <si>
-    <t>3*Fe_g, 2*O2</t>
-  </si>
-  <si>
     <t>1*Ca, 1*O</t>
   </si>
   <si>
-    <t>1*Ca_g, 0.5*O2</t>
-  </si>
-  <si>
     <t>2*Al, 3*O</t>
   </si>
   <si>
@@ -640,6 +625,27 @@
   </si>
   <si>
     <t>2*K</t>
+  </si>
+  <si>
+    <t>1*Ca, 0.5*O2</t>
+  </si>
+  <si>
+    <t>1*Fe</t>
+  </si>
+  <si>
+    <t>1*Fe, 0.5*O2</t>
+  </si>
+  <si>
+    <t>2*Fe, 1.5*O2</t>
+  </si>
+  <si>
+    <t>3*Fe, 2*O2</t>
+  </si>
+  <si>
+    <t>1*Na</t>
+  </si>
+  <si>
+    <t>1*K</t>
   </si>
 </sst>
 </file>
@@ -2976,7 +2982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1716CC3-50ED-4F4B-B9E3-816FAA8C5A11}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
@@ -3149,7 +3155,7 @@
         <v>19704</v>
       </c>
       <c r="E10" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -3166,7 +3172,7 @@
         <v>9753</v>
       </c>
       <c r="E11" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -3185,7 +3191,7 @@
         <v>75643.0936141329</v>
       </c>
       <c r="E12" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -3204,7 +3210,7 @@
         <v>111052.62061396299</v>
       </c>
       <c r="E13" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -3221,7 +3227,7 @@
         <v>49586</v>
       </c>
       <c r="E14" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -3238,7 +3244,7 @@
         <v>6128</v>
       </c>
       <c r="E15" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -3255,7 +3261,7 @@
         <v>153255</v>
       </c>
       <c r="E16" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -3272,7 +3278,7 @@
         <v>15862</v>
       </c>
       <c r="E17" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -3289,7 +3295,7 @@
         <v>13719</v>
       </c>
       <c r="E18" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -3306,7 +3312,7 @@
         <v>41956</v>
       </c>
       <c r="E19" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -3323,7 +3329,7 @@
         <v>15867.5</v>
       </c>
       <c r="E20" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -3340,7 +3346,7 @@
         <v>54745</v>
       </c>
       <c r="E21" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -3357,7 +3363,7 @@
         <v>23025</v>
       </c>
       <c r="E22" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -3374,7 +3380,7 @@
         <v>-2101</v>
       </c>
       <c r="E23" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -3391,7 +3397,7 @@
         <v>95362</v>
       </c>
       <c r="E24" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -3408,7 +3414,7 @@
         <v>17926</v>
       </c>
       <c r="E25" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -3425,7 +3431,7 @@
         <v>40286</v>
       </c>
       <c r="E26" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -3442,7 +3448,7 @@
         <v>14569</v>
       </c>
       <c r="E27" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -3459,7 +3465,7 @@
         <v>4281</v>
       </c>
       <c r="E28" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -3476,7 +3482,7 @@
         <v>25180</v>
       </c>
       <c r="E29" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -3492,6 +3498,9 @@
       <c r="D30">
         <v>-27851</v>
       </c>
+      <c r="E30" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -3507,7 +3516,7 @@
         <v>36735</v>
       </c>
       <c r="E31" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -3524,7 +3533,7 @@
         <v>14241</v>
       </c>
       <c r="E32" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -3541,7 +3550,7 @@
         <v>44099</v>
       </c>
       <c r="E33" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -3558,7 +3567,7 @@
         <v>2852</v>
       </c>
       <c r="E34" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -3573,6 +3582,9 @@
       </c>
       <c r="D35">
         <v>-23760</v>
+      </c>
+      <c r="E35" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added stuff to report.py
</commit_message>
<xml_diff>
--- a/data/MAGMA_Thermodynamic_Data.xlsx
+++ b/data/MAGMA_Thermodynamic_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Documents\MAGMApy\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/PycharmProjects/MAGMApy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86AE9BDA-ED28-4FEC-84EF-36F1F983BC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0DA627-5993-0F43-97A3-E4553B8E05ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20685" yWindow="435" windowWidth="27915" windowHeight="19665" activeTab="2" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
+    <workbookView xWindow="16680" yWindow="1140" windowWidth="28800" windowHeight="15960" activeTab="2" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="205">
   <si>
     <t>R1</t>
   </si>
@@ -652,36 +652,6 @@
   </si>
   <si>
     <t>K40</t>
-  </si>
-  <si>
-    <t>ZnO</t>
-  </si>
-  <si>
-    <t>Zn</t>
-  </si>
-  <si>
-    <t>Zn2SiO4</t>
-  </si>
-  <si>
-    <t>ZnTiO3</t>
-  </si>
-  <si>
-    <t>Zn2TiO4</t>
-  </si>
-  <si>
-    <t>ZnAl2O4</t>
-  </si>
-  <si>
-    <t>K41</t>
-  </si>
-  <si>
-    <t>K42</t>
-  </si>
-  <si>
-    <t>K43</t>
-  </si>
-  <si>
-    <t>K44</t>
   </si>
 </sst>
 </file>
@@ -1039,15 +1009,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA51B45C-F7CC-3B41-AC8C-EF614A95CDBA}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1073,7 +1043,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1069,7 @@
         <v>-94311</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1125,7 +1095,7 @@
         <v>-46992</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1151,7 +1121,7 @@
         <v>-44992</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1177,7 +1147,7 @@
         <v>-49586</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1203,7 +1173,7 @@
         <v>-153255</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1229,7 +1199,7 @@
         <v>-95362</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1255,7 +1225,7 @@
         <v>-40286</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1281,7 +1251,7 @@
         <v>-36735</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1307,7 +1277,7 @@
         <v>-112807</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1333,7 +1303,7 @@
         <v>-100627</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1357,32 +1327,6 @@
       </c>
       <c r="H12">
         <v>-91886</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>206</v>
-      </c>
-      <c r="C13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
-        <v>205</v>
-      </c>
-      <c r="G13">
-        <v>14.32</v>
-      </c>
-      <c r="H13">
-        <v>-35990.589999999997</v>
       </c>
     </row>
   </sheetData>
@@ -1395,14 +1339,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB38BCC-BF73-D341-9EF2-69884C8E8DA9}">
   <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomLeft" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1452,7 +1396,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1469,7 +1413,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1486,7 +1430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1506,7 +1450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1526,7 +1470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1543,7 +1487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1563,7 +1507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1580,7 +1524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1601,7 +1545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1621,7 +1565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1638,7 +1582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1658,7 +1602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1675,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1695,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1715,7 +1659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1735,7 +1679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1755,7 +1699,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1772,7 +1716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1792,7 +1736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1812,7 +1756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1829,7 +1773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1849,7 +1793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1866,7 +1810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1886,7 +1830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1903,7 +1847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1923,7 +1867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1940,7 +1884,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1960,7 +1904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1977,7 +1921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1997,7 +1941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2017,7 +1961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2034,7 +1978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2054,7 +1998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2074,7 +2018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2094,7 +2038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2111,7 +2055,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2131,7 +2075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -2151,7 +2095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -2176,16 +2120,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575B768E-B263-7849-9255-8DC0D8CFF25A}">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I46" sqref="I46"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2222,11 +2166,8 @@
       <c r="L1" t="s">
         <v>81</v>
       </c>
-      <c r="M1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2246,7 +2187,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2266,7 +2207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2286,7 +2227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2306,7 +2247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2326,7 +2267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2346,7 +2287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2366,7 +2307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2386,7 +2327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2406,7 +2347,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2426,7 +2367,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2446,7 +2387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2469,7 +2410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2492,7 +2433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2515,7 +2456,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2538,7 +2479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2558,7 +2499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2578,7 +2519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2601,7 +2542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2621,7 +2562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2641,7 +2582,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2661,7 +2602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2681,7 +2622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2704,7 +2645,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2724,7 +2665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2744,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2767,7 +2708,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2790,7 +2731,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2810,7 +2751,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2830,7 +2771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2853,7 +2794,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2873,7 +2814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2893,7 +2834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2916,7 +2857,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2939,7 +2880,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2959,7 +2900,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2982,7 +2923,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -3008,7 +2949,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -3028,7 +2969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>136</v>
       </c>
@@ -3036,62 +2977,12 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>204</v>
       </c>
       <c r="B41" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>211</v>
-      </c>
-      <c r="B42" t="s">
-        <v>207</v>
-      </c>
-      <c r="M42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>212</v>
-      </c>
-      <c r="B43" t="s">
-        <v>208</v>
-      </c>
-      <c r="E43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>213</v>
-      </c>
-      <c r="B44" t="s">
-        <v>209</v>
-      </c>
-      <c r="J44">
-        <v>1</v>
-      </c>
-      <c r="M44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>214</v>
-      </c>
-      <c r="B45" t="s">
-        <v>210</v>
-      </c>
-      <c r="I45">
-        <v>1</v>
-      </c>
-      <c r="M45">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3105,13 +2996,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1716CC3-50ED-4F4B-B9E3-816FAA8C5A11}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -3128,7 +3019,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>168</v>
       </c>
@@ -3145,7 +3036,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3162,7 +3053,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3179,7 +3070,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3196,7 +3087,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3213,7 +3104,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -3230,7 +3121,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -3247,7 +3138,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3264,7 +3155,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -3281,7 +3172,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -3298,7 +3189,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -3317,7 +3208,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3336,7 +3227,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3353,7 +3244,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3370,7 +3261,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3387,7 +3278,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -3404,7 +3295,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3421,7 +3312,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3438,7 +3329,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3455,7 +3346,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3472,7 +3363,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3489,7 +3380,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -3506,7 +3397,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -3523,7 +3414,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -3540,7 +3431,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -3557,7 +3448,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -3574,7 +3465,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -3591,7 +3482,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -3608,7 +3499,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -3625,7 +3516,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -3642,7 +3533,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -3659,7 +3550,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -3676,7 +3567,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -3693,7 +3584,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Working match between MAGMA SiO2 and my own in K_from_Gibbs.py
</commit_message>
<xml_diff>
--- a/data/MAGMA_Thermodynamic_Data.xlsx
+++ b/data/MAGMA_Thermodynamic_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/PycharmProjects/MAGMApy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/Documents - Scott’s MacBook Pro/PhD Research/MAGMApy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0DA627-5993-0F43-97A3-E4553B8E05ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF42816-F382-9D45-987B-B51165638C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16680" yWindow="1140" windowWidth="28800" windowHeight="15960" activeTab="2" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
+    <workbookView xWindow="14040" yWindow="760" windowWidth="20520" windowHeight="21580" activeTab="3" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="224">
   <si>
     <t>R1</t>
   </si>
@@ -652,6 +652,63 @@
   </si>
   <si>
     <t>K40</t>
+  </si>
+  <si>
+    <t>Zn</t>
+  </si>
+  <si>
+    <t>ZnO</t>
+  </si>
+  <si>
+    <t>R39</t>
+  </si>
+  <si>
+    <t>ZnO_g</t>
+  </si>
+  <si>
+    <t>1*Zn, 1*O</t>
+  </si>
+  <si>
+    <t>K41</t>
+  </si>
+  <si>
+    <t>K42</t>
+  </si>
+  <si>
+    <t>K43</t>
+  </si>
+  <si>
+    <t>K44</t>
+  </si>
+  <si>
+    <t>Zn2SiO4</t>
+  </si>
+  <si>
+    <t>ZnTiO3</t>
+  </si>
+  <si>
+    <t>Zn2TiO4</t>
+  </si>
+  <si>
+    <t>ZnAl2O4</t>
+  </si>
+  <si>
+    <t>Zn_liq</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>Zn_l</t>
+  </si>
+  <si>
+    <t>1*Zn</t>
+  </si>
+  <si>
+    <t>ZnO_l</t>
+  </si>
+  <si>
+    <t>1*Zn, 0.5*O2</t>
   </si>
 </sst>
 </file>
@@ -1009,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA51B45C-F7CC-3B41-AC8C-EF614A95CDBA}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1327,6 +1384,32 @@
       </c>
       <c r="H12">
         <v>-91886</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>205</v>
+      </c>
+      <c r="C13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G13">
+        <v>12.02455</v>
+      </c>
+      <c r="H13">
+        <v>33554.101999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1337,16 +1420,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB38BCC-BF73-D341-9EF2-69884C8E8DA9}">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:D1"/>
+      <selection pane="bottomLeft" activeCell="Q41" sqref="Q41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1395,8 +1478,11 @@
       <c r="P1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1413,7 +1499,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1430,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1450,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1470,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1487,7 +1573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1507,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1524,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1545,7 +1631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1565,7 +1651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1582,7 +1668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1602,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1619,7 +1705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1639,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1659,7 +1745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1978,7 +2064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1998,7 +2084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2018,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2038,7 +2124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2055,7 +2141,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2075,7 +2161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -2095,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -2109,6 +2195,40 @@
         <v>0</v>
       </c>
       <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>207</v>
+      </c>
+      <c r="B40" t="s">
+        <v>205</v>
+      </c>
+      <c r="C40">
+        <v>5.1891999999999996</v>
+      </c>
+      <c r="D40">
+        <v>-6124.14</v>
+      </c>
+      <c r="Q40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>219</v>
+      </c>
+      <c r="B41" t="s">
+        <v>206</v>
+      </c>
+      <c r="C41">
+        <v>3.1945999999999999</v>
+      </c>
+      <c r="D41">
+        <v>10967.931</v>
+      </c>
+      <c r="Q41">
         <v>1</v>
       </c>
     </row>
@@ -2120,16 +2240,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575B768E-B263-7849-9255-8DC0D8CFF25A}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2166,8 +2286,11 @@
       <c r="L1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2187,7 +2310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2207,7 +2330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2227,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2247,7 +2370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2267,7 +2390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2287,7 +2410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2307,7 +2430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2327,7 +2450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2347,7 +2470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2367,7 +2490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2387,7 +2510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2410,7 +2533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2433,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2456,7 +2579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2814,7 +2937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2834,7 +2957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2857,7 +2980,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2880,7 +3003,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2900,7 +3023,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2923,7 +3046,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -2949,7 +3072,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -2969,7 +3092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>136</v>
       </c>
@@ -2977,12 +3100,92 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>204</v>
       </c>
       <c r="B41" t="s">
         <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>210</v>
+      </c>
+      <c r="B42" t="s">
+        <v>214</v>
+      </c>
+      <c r="C42">
+        <v>0.59599999999999997</v>
+      </c>
+      <c r="D42">
+        <v>1777.9</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>211</v>
+      </c>
+      <c r="B43" t="s">
+        <v>215</v>
+      </c>
+      <c r="C43">
+        <v>2.7930000000000001</v>
+      </c>
+      <c r="D43">
+        <v>-5625.5439999999999</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>212</v>
+      </c>
+      <c r="B44" t="s">
+        <v>216</v>
+      </c>
+      <c r="C44">
+        <v>-0.1464</v>
+      </c>
+      <c r="D44">
+        <v>3044.1203</v>
+      </c>
+      <c r="J44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>213</v>
+      </c>
+      <c r="B45" t="s">
+        <v>217</v>
+      </c>
+      <c r="C45">
+        <v>-1.27715</v>
+      </c>
+      <c r="D45">
+        <v>4727.51</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2994,10 +3197,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1716CC3-50ED-4F4B-B9E3-816FAA8C5A11}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3524,10 +3727,10 @@
         <v>159</v>
       </c>
       <c r="C31">
-        <v>-15.33</v>
+        <v>-15.21</v>
       </c>
       <c r="D31">
-        <v>36735</v>
+        <v>36404</v>
       </c>
       <c r="E31" t="s">
         <v>193</v>
@@ -3541,10 +3744,10 @@
         <v>160</v>
       </c>
       <c r="C32">
-        <v>-4.75</v>
+        <v>-4.5888</v>
       </c>
       <c r="D32">
-        <v>14241</v>
+        <v>14548.7</v>
       </c>
       <c r="E32" t="s">
         <v>194</v>
@@ -3558,10 +3761,10 @@
         <v>161</v>
       </c>
       <c r="C33">
-        <v>-14.204000000000001</v>
+        <v>-10.741099999999999</v>
       </c>
       <c r="D33">
-        <v>44099</v>
+        <v>26600.3</v>
       </c>
       <c r="E33" t="s">
         <v>193</v>
@@ -3599,6 +3802,57 @@
       </c>
       <c r="E35" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36">
+        <v>3.1945999999999999</v>
+      </c>
+      <c r="D36">
+        <v>-10967.931</v>
+      </c>
+      <c r="E36" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" t="s">
+        <v>222</v>
+      </c>
+      <c r="C37">
+        <v>-12.02455</v>
+      </c>
+      <c r="D37">
+        <v>33554.101999999999</v>
+      </c>
+      <c r="E37" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" t="s">
+        <v>220</v>
+      </c>
+      <c r="C38">
+        <v>-5.1891999999999996</v>
+      </c>
+      <c r="D38">
+        <v>6124.14</v>
+      </c>
+      <c r="E38" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added advanced oxygen fugacity support.
</commit_message>
<xml_diff>
--- a/data/MAGMA_Thermodynamic_Data.xlsx
+++ b/data/MAGMA_Thermodynamic_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scotthull/Documents - Scott’s MacBook Pro/PhD Research/MAGMApy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\Documents\MAGMApy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF42816-F382-9D45-987B-B51165638C55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2736AD95-1455-4385-A802-648F009EB0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14040" yWindow="760" windowWidth="20520" windowHeight="21580" activeTab="3" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
+    <workbookView xWindow="3135" yWindow="135" windowWidth="10305" windowHeight="20985" firstSheet="1" activeTab="3" xr2:uid="{456E65B5-CD77-6C45-B868-846F4563A2B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="3" r:id="rId1"/>
@@ -1069,12 +1069,12 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>-94311</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>-46992</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>-44992</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>-49586</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>-153255</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>-95362</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>-40286</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1302,13 +1302,13 @@
         <v>81</v>
       </c>
       <c r="G9">
-        <v>15.33</v>
+        <v>-15.21</v>
       </c>
       <c r="H9">
-        <v>-36735</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>36404</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>-112807</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>-100627</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>-91886</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1424,12 +1424,12 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q41" sqref="Q41"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1970,7 +1970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2141,7 +2141,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>207</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>219</v>
       </c>
@@ -2247,9 +2247,9 @@
       <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2533,7 +2533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2556,7 +2556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2642,7 +2642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2788,7 +2788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2980,7 +2980,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>136</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>204</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>210</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>211</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>212</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>213</v>
       </c>
@@ -3199,13 +3199,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1716CC3-50ED-4F4B-B9E3-816FAA8C5A11}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -3222,7 +3222,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>168</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3549,7 +3549,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -3634,7 +3634,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -3651,7 +3651,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -3685,7 +3685,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -3753,7 +3753,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -3804,7 +3804,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Attempting to impose saturation conditions on P_i.
</commit_message>
<xml_diff>
--- a/data/MAGMA_Thermodynamic_Data.xlsx
+++ b/data/MAGMA_Thermodynamic_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Scott\PycharmProjects\MAGMApy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1D6DF5-BDDE-47AC-937C-3F7E852C6022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F200DFB1-E7F2-443F-A7BE-856620C17C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21615" windowHeight="16920" activeTab="3" xr2:uid="{A66FC4F3-F169-E14C-B2AF-C9A0F5AF27FB}"/>
+    <workbookView xWindow="-21570" yWindow="4395" windowWidth="21615" windowHeight="16920" activeTab="3" xr2:uid="{A66FC4F3-F169-E14C-B2AF-C9A0F5AF27FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="242">
   <si>
     <t>Label</t>
   </si>
@@ -759,6 +759,9 @@
   </si>
   <si>
     <t>1*Zn</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
   <si>
     <t>1*Zn_l, 0.5*O2</t>
@@ -1119,15 +1122,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5476373E-24FC-B041-9BEB-C58A30D18A9B}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1152,8 +1155,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1173,13 +1179,16 @@
         <v>11</v>
       </c>
       <c r="G2">
-        <v>22.13</v>
+        <v>23.278899717000002</v>
       </c>
       <c r="H2">
-        <v>-94311</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>-99057.305063000007</v>
+      </c>
+      <c r="I2">
+        <v>2655395.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1205,7 +1214,7 @@
         <v>-46992</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1231,7 +1240,7 @@
         <v>-44992</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1257,7 +1266,7 @@
         <v>-49586</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1283,7 +1292,7 @@
         <v>-153255</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1309,7 +1318,7 @@
         <v>-95362</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1335,7 +1344,7 @@
         <v>-40286</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1361,7 +1370,7 @@
         <v>36404</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1381,13 +1390,13 @@
         <v>35</v>
       </c>
       <c r="G10">
-        <v>9.5500000000000007</v>
+        <v>-9.5500000000000007</v>
       </c>
       <c r="H10">
-        <v>-63948</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63948</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1407,13 +1416,13 @@
         <v>38</v>
       </c>
       <c r="G11">
-        <v>19.18</v>
+        <v>-26.91</v>
       </c>
       <c r="H11">
-        <v>-100627</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>204359</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1433,13 +1442,13 @@
         <v>41</v>
       </c>
       <c r="G12">
-        <v>18.670000000000002</v>
+        <v>-29.86</v>
       </c>
       <c r="H12">
-        <v>-91886</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>200903</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1462,7 +1471,7 @@
         <v>12.02455</v>
       </c>
       <c r="H13">
-        <v>33554.101999999999</v>
+        <v>-33554.101999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1475,7 +1484,7 @@
   <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2411,6 +2420,9 @@
       </c>
       <c r="E41">
         <v>-10967.931</v>
+      </c>
+      <c r="F41">
+        <v>0.5</v>
       </c>
       <c r="U41">
         <v>1</v>
@@ -2427,8 +2439,8 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2482,10 +2494,10 @@
         <v>115</v>
       </c>
       <c r="C2">
-        <v>-0.94</v>
+        <v>-0.94840000000000002</v>
       </c>
       <c r="D2">
-        <v>7434</v>
+        <v>7404.5</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2502,10 +2514,10 @@
         <v>116</v>
       </c>
       <c r="C3">
-        <v>0.42</v>
+        <v>0.41520000000000001</v>
       </c>
       <c r="D3">
-        <v>2329</v>
+        <v>2330.6170000000002</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -3414,15 +3426,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E18122-6D19-724B-BF5D-00F815E4C0D4}">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3436,10 +3448,13 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>170</v>
       </c>
@@ -3452,11 +3467,11 @@
       <c r="D2">
         <v>-13282</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3464,16 +3479,20 @@
         <v>172</v>
       </c>
       <c r="C3">
-        <v>-11.7</v>
+        <v>-12.8489</v>
       </c>
       <c r="D3">
-        <v>38621</v>
-      </c>
-      <c r="E3" t="s">
+        <v>43367.3</v>
+      </c>
+      <c r="E3">
+        <f>-2655400</f>
+        <v>-2655400</v>
+      </c>
+      <c r="F3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3486,11 +3505,11 @@
       <c r="D4">
         <v>-8207</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -3503,11 +3522,11 @@
       <c r="D5">
         <v>19892.900000000001</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -3520,11 +3539,11 @@
       <c r="D6">
         <v>-20919</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -3537,11 +3556,11 @@
       <c r="D7">
         <v>-3794</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -3554,11 +3573,11 @@
       <c r="D8">
         <v>46992</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -3571,11 +3590,11 @@
       <c r="D9">
         <v>44992</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -3588,11 +3607,11 @@
       <c r="D10">
         <v>19704</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -3605,11 +3624,11 @@
       <c r="D11">
         <v>9753</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -3624,11 +3643,11 @@
         <f>75643.0936141329</f>
         <v>75643.0936141329</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -3643,11 +3662,11 @@
         <f>111052.620613963</f>
         <v>111052.62061396299</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -3660,11 +3679,11 @@
       <c r="D14">
         <v>49586</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -3677,11 +3696,11 @@
       <c r="D15">
         <v>6128</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -3694,11 +3713,11 @@
       <c r="D16">
         <v>153255</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -3711,11 +3730,11 @@
       <c r="D17">
         <v>15862</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -3728,11 +3747,11 @@
       <c r="D18">
         <v>13719</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -3745,11 +3764,11 @@
       <c r="D19">
         <v>41956</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -3762,11 +3781,11 @@
       <c r="D20">
         <v>15867.5</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -3779,11 +3798,11 @@
       <c r="D21">
         <v>54745</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -3796,11 +3815,11 @@
       <c r="D22">
         <v>23025</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -3813,11 +3832,11 @@
       <c r="D23">
         <v>-2101</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -3830,11 +3849,11 @@
       <c r="D24">
         <v>95362</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -3847,11 +3866,11 @@
       <c r="D25">
         <v>17926</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -3864,11 +3883,11 @@
       <c r="D26">
         <v>40286</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -3881,11 +3900,11 @@
       <c r="D27">
         <v>13305.8712</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -3898,11 +3917,11 @@
       <c r="D28">
         <v>4281</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>84</v>
       </c>
@@ -3915,11 +3934,11 @@
       <c r="D29">
         <v>25351.16747</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -3932,11 +3951,11 @@
       <c r="D30">
         <v>-27851</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>86</v>
       </c>
@@ -3949,11 +3968,11 @@
       <c r="D31">
         <v>36404</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -3966,11 +3985,11 @@
       <c r="D32">
         <v>14548.7</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>89</v>
       </c>
@@ -3983,11 +4002,11 @@
       <c r="D33">
         <v>26600.3</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>90</v>
       </c>
@@ -4000,11 +4019,11 @@
       <c r="D34">
         <v>2852</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>92</v>
       </c>
@@ -4017,11 +4036,11 @@
       <c r="D35">
         <v>-23760</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>93</v>
       </c>
@@ -4034,11 +4053,11 @@
       <c r="D36">
         <v>-10967.931</v>
       </c>
-      <c r="E36" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>95</v>
       </c>
@@ -4051,11 +4070,11 @@
       <c r="D37">
         <v>33554.101999999999</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>96</v>
       </c>
@@ -4068,7 +4087,7 @@
       <c r="D38">
         <v>6124.14</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>239</v>
       </c>
     </row>

</xml_diff>